<commit_message>
Added "add new customer" functionality. Receiving errors when adding customer.
</commit_message>
<xml_diff>
--- a/UML.xlsx
+++ b/UML.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\OneDrive\Documents\School\WGU\Term 6\Software II\Scheduler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9ba3bea643936b3e/Documents/School/WGU/Term 6/Software II/Scheduler/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="50" documentId="E1FC892FEA21F6556586FE291B423042DC87A56C" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{F9849742-AB10-4AD2-8F28-6D1A167CE98E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8150"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="86">
   <si>
     <t>MainApp</t>
   </si>
@@ -226,12 +227,69 @@
   </si>
   <si>
     <t>Office</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>addressId: int</t>
+  </si>
+  <si>
+    <t>address: String</t>
+  </si>
+  <si>
+    <t>address2: String</t>
+  </si>
+  <si>
+    <t>cityID: int</t>
+  </si>
+  <si>
+    <t>postalCode: String</t>
+  </si>
+  <si>
+    <t>phone: String</t>
+  </si>
+  <si>
+    <t>createdBy: String</t>
+  </si>
+  <si>
+    <t>lastUpdate: dateTime</t>
+  </si>
+  <si>
+    <t>createDate: dateTime</t>
+  </si>
+  <si>
+    <t>lastUpdateBy: String</t>
+  </si>
+  <si>
+    <t>set*()</t>
+  </si>
+  <si>
+    <t>get*()</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>cityId: int</t>
+  </si>
+  <si>
+    <t>city: String</t>
+  </si>
+  <si>
+    <t>countryId: int</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>country: String</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -857,158 +915,285 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+    <row r="3" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="D6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="D7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="13" t="s">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="D8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E8" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="D9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="13" t="s">
+    <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="D10" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="14" t="s">
+    <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="8" t="s">
+    <row r="12" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="E12" s="8" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B19" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B20" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B21" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B22" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B23" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B24" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B27" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B28" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B29" s="8" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1018,7 +1203,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>